<commit_message>
OFC Nations Cup 2004, 2008
OFC Nations Cup 2004, 2008
</commit_message>
<xml_diff>
--- a/Scripts/ofcnationscup/ofcnationscup.xlsx
+++ b/Scripts/ofcnationscup/ofcnationscup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="472" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="472" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="1973" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,15 @@
     <sheet name="1998" sheetId="4" r:id="rId4"/>
     <sheet name="2000" sheetId="5" r:id="rId5"/>
     <sheet name="2002" sheetId="6" r:id="rId6"/>
+    <sheet name="2004" sheetId="7" r:id="rId7"/>
+    <sheet name="2008" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="14">
   <si>
     <t>id</t>
   </si>
@@ -7683,7 +7685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10021,4 +10023,3743 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G88"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="111.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="str">
+        <f>"insert into game (matchid, matchdate, game_type, country) values (" &amp; A1 &amp; ", '" &amp; B1 &amp; "', " &amp; C1 &amp; ", " &amp; D1 &amp;  ");"</f>
+        <v>insert into game (matchid, matchdate, game_type, country) values (matchid, 'matchdate', game_type, country);</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <f>'2002'!A27 + 1</f>
+        <v>69</v>
+      </c>
+      <c r="B2" s="2" t="str">
+        <f>"2004-05-29"</f>
+        <v>2004-05-29</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>61</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G18" si="0">"insert into game (matchid, matchdate, game_type, country) values (" &amp; A2 &amp; ", '" &amp; B2 &amp; "', " &amp; C2 &amp; ", " &amp; D2 &amp;  ");"</f>
+        <v>insert into game (matchid, matchdate, game_type, country) values (69, '2004-05-29', 2, 61);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>70</v>
+      </c>
+      <c r="B3" s="2" t="str">
+        <f>"2004-05-29"</f>
+        <v>2004-05-29</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <f>D2</f>
+        <v>61</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (70, '2004-05-29', 2, 61);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A18" si="1">A3+1</f>
+        <v>71</v>
+      </c>
+      <c r="B4" s="2" t="str">
+        <f>"2004-05-29"</f>
+        <v>2004-05-29</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D18" si="2">D3</f>
+        <v>61</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (71, '2004-05-29', 2, 61);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="B5" s="2" t="str">
+        <f>"2004-05-31"</f>
+        <v>2004-05-31</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="2"/>
+        <v>61</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (72, '2004-05-31', 2, 61);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="B6" s="2" t="str">
+        <f>"2004-05-31"</f>
+        <v>2004-05-31</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="2"/>
+        <v>61</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (73, '2004-05-31', 2, 61);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="B7" s="2" t="str">
+        <f>"2004-05-31"</f>
+        <v>2004-05-31</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>61</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (74, '2004-05-31', 2, 61);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="B8" s="2" t="str">
+        <f>"2004-06-02"</f>
+        <v>2004-06-02</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>61</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (75, '2004-06-02', 2, 61);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="B9" s="2" t="str">
+        <f>"2004-06-02"</f>
+        <v>2004-06-02</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>61</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (76, '2004-06-02', 2, 61);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+      <c r="B10" s="2" t="str">
+        <f>"2004-06-02"</f>
+        <v>2004-06-02</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>61</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (77, '2004-06-02', 2, 61);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="B11" s="2" t="str">
+        <f>"2004-06-04"</f>
+        <v>2004-06-04</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>61</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (78, '2004-06-04', 2, 61);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="B12" s="2" t="str">
+        <f>"2004-06-04"</f>
+        <v>2004-06-04</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>61</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (79, '2004-06-04', 2, 61);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="B13" s="2" t="str">
+        <f>"2004-06-04"</f>
+        <v>2004-06-04</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>61</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (80, '2004-06-04', 2, 61);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="B14" s="2" t="str">
+        <f>"2004-06-06"</f>
+        <v>2004-06-06</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="2"/>
+        <v>61</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (81, '2004-06-06', 2, 61);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="B15" s="2" t="str">
+        <f>"2004-06-06"</f>
+        <v>2004-06-06</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>61</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (82, '2004-06-06', 2, 61);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+      <c r="B16" s="2" t="str">
+        <f>"2004-06-06"</f>
+        <v>2004-06-06</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="2"/>
+        <v>61</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (83, '2004-06-06', 2, 61);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="B17" s="2" t="str">
+        <f>"2004-10-12"</f>
+        <v>2004-10-12</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>677</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (84, '2004-10-12', 6, 677);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="B18" s="2" t="str">
+        <f>"2004-10-12"</f>
+        <v>2004-10-12</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>61</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (85, '2004-10-12', 6, 61);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" t="str">
+        <f>"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A20 &amp; ", " &amp; B20 &amp; ", " &amp; C20 &amp; ", " &amp; D20 &amp; ", " &amp; E20 &amp; ", " &amp; F20 &amp; ");"</f>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (id, matchid, squad, goals, points, time_type);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <f>'2002'!A97 + 1</f>
+        <v>277</v>
+      </c>
+      <c r="B21" s="3">
+        <f>A2</f>
+        <v>69</v>
+      </c>
+      <c r="C21" s="3">
+        <v>678</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <v>2</v>
+      </c>
+      <c r="G21" s="3" t="str">
+        <f t="shared" ref="G21:G44" si="3">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A21 &amp; ", " &amp; B21 &amp; ", " &amp; C21 &amp; ", " &amp; D21 &amp; ", " &amp; E21 &amp; ", " &amp; F21 &amp; ");"</f>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (277, 69, 678, 0, 0, 2);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <f>A21+1</f>
+        <v>278</v>
+      </c>
+      <c r="B22" s="3">
+        <f>B21</f>
+        <v>69</v>
+      </c>
+      <c r="C22" s="3">
+        <v>678</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
+        <v>1</v>
+      </c>
+      <c r="G22" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (278, 69, 678, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <f t="shared" ref="A23:A28" si="4">A22+1</f>
+        <v>279</v>
+      </c>
+      <c r="B23" s="3">
+        <f>B21</f>
+        <v>69</v>
+      </c>
+      <c r="C23" s="3">
+        <v>677</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1</v>
+      </c>
+      <c r="E23" s="3">
+        <v>3</v>
+      </c>
+      <c r="F23" s="3">
+        <v>2</v>
+      </c>
+      <c r="G23" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (279, 69, 677, 1, 3, 2);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <f t="shared" si="4"/>
+        <v>280</v>
+      </c>
+      <c r="B24" s="3">
+        <f>B21</f>
+        <v>69</v>
+      </c>
+      <c r="C24" s="3">
+        <v>677</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
+        <v>1</v>
+      </c>
+      <c r="G24" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (280, 69, 677, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="4"/>
+        <v>281</v>
+      </c>
+      <c r="B25">
+        <f>B21+1</f>
+        <v>70</v>
+      </c>
+      <c r="C25" s="4">
+        <v>689</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0</v>
+      </c>
+      <c r="E25" s="5">
+        <v>1</v>
+      </c>
+      <c r="F25" s="4">
+        <v>2</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (281, 70, 689, 0, 1, 2);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="4"/>
+        <v>282</v>
+      </c>
+      <c r="B26">
+        <f>B25</f>
+        <v>70</v>
+      </c>
+      <c r="C26" s="4">
+        <v>689</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0</v>
+      </c>
+      <c r="E26" s="5">
+        <v>0</v>
+      </c>
+      <c r="F26" s="4">
+        <v>1</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (282, 70, 689, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="4"/>
+        <v>283</v>
+      </c>
+      <c r="B27">
+        <f>B25</f>
+        <v>70</v>
+      </c>
+      <c r="C27" s="4">
+        <v>679</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0</v>
+      </c>
+      <c r="E27" s="5">
+        <v>1</v>
+      </c>
+      <c r="F27" s="4">
+        <v>2</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (283, 70, 679, 0, 1, 2);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="4"/>
+        <v>284</v>
+      </c>
+      <c r="B28">
+        <f>B25</f>
+        <v>70</v>
+      </c>
+      <c r="C28" s="4">
+        <v>679</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0</v>
+      </c>
+      <c r="E28" s="5">
+        <v>0</v>
+      </c>
+      <c r="F28" s="4">
+        <v>1</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (284, 70, 679, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <f>A28+1</f>
+        <v>285</v>
+      </c>
+      <c r="B29" s="3">
+        <f>B25+1</f>
+        <v>71</v>
+      </c>
+      <c r="C29" s="3">
+        <v>61</v>
+      </c>
+      <c r="D29" s="3">
+        <v>1</v>
+      </c>
+      <c r="E29" s="3">
+        <v>3</v>
+      </c>
+      <c r="F29" s="3">
+        <v>2</v>
+      </c>
+      <c r="G29" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (285, 71, 61, 1, 3, 2);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <f>A29+1</f>
+        <v>286</v>
+      </c>
+      <c r="B30" s="3">
+        <f>B29</f>
+        <v>71</v>
+      </c>
+      <c r="C30" s="3">
+        <v>61</v>
+      </c>
+      <c r="D30" s="3">
+        <v>1</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0</v>
+      </c>
+      <c r="F30" s="3">
+        <v>1</v>
+      </c>
+      <c r="G30" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (286, 71, 61, 1, 0, 1);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <f>A30+1</f>
+        <v>287</v>
+      </c>
+      <c r="B31" s="3">
+        <f>B29</f>
+        <v>71</v>
+      </c>
+      <c r="C31" s="3">
+        <v>64</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0</v>
+      </c>
+      <c r="F31" s="3">
+        <v>2</v>
+      </c>
+      <c r="G31" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (287, 71, 64, 0, 0, 2);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <f>A31+1</f>
+        <v>288</v>
+      </c>
+      <c r="B32" s="3">
+        <f>B29</f>
+        <v>71</v>
+      </c>
+      <c r="C32" s="3">
+        <v>64</v>
+      </c>
+      <c r="D32" s="3">
+        <v>0</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0</v>
+      </c>
+      <c r="F32" s="3">
+        <v>1</v>
+      </c>
+      <c r="G32" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (288, 71, 64, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <f>A32+1</f>
+        <v>289</v>
+      </c>
+      <c r="B33">
+        <f>B29+1</f>
+        <v>72</v>
+      </c>
+      <c r="C33" s="4">
+        <v>64</v>
+      </c>
+      <c r="D33" s="4">
+        <v>3</v>
+      </c>
+      <c r="E33" s="5">
+        <v>3</v>
+      </c>
+      <c r="F33" s="4">
+        <v>2</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (289, 72, 64, 3, 3, 2);</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <f t="shared" ref="A34:A88" si="5">A33+1</f>
+        <v>290</v>
+      </c>
+      <c r="B34">
+        <f>B33</f>
+        <v>72</v>
+      </c>
+      <c r="C34" s="4">
+        <v>64</v>
+      </c>
+      <c r="D34" s="4">
+        <v>1</v>
+      </c>
+      <c r="E34" s="5">
+        <v>0</v>
+      </c>
+      <c r="F34" s="4">
+        <v>1</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (290, 72, 64, 1, 0, 1);</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <f t="shared" si="5"/>
+        <v>291</v>
+      </c>
+      <c r="B35">
+        <f>B33</f>
+        <v>72</v>
+      </c>
+      <c r="C35" s="4">
+        <v>677</v>
+      </c>
+      <c r="D35" s="4">
+        <v>0</v>
+      </c>
+      <c r="E35" s="5">
+        <v>0</v>
+      </c>
+      <c r="F35" s="4">
+        <v>2</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (291, 72, 677, 0, 0, 2);</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <f t="shared" si="5"/>
+        <v>292</v>
+      </c>
+      <c r="B36">
+        <f>B33</f>
+        <v>72</v>
+      </c>
+      <c r="C36" s="4">
+        <v>677</v>
+      </c>
+      <c r="D36" s="4">
+        <v>0</v>
+      </c>
+      <c r="E36" s="5">
+        <v>0</v>
+      </c>
+      <c r="F36" s="4">
+        <v>1</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (292, 72, 677, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <f t="shared" si="5"/>
+        <v>293</v>
+      </c>
+      <c r="B37" s="3">
+        <f>B33+1</f>
+        <v>73</v>
+      </c>
+      <c r="C37" s="3">
+        <v>61</v>
+      </c>
+      <c r="D37" s="3">
+        <v>9</v>
+      </c>
+      <c r="E37" s="3">
+        <v>3</v>
+      </c>
+      <c r="F37" s="3">
+        <v>2</v>
+      </c>
+      <c r="G37" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (293, 73, 61, 9, 3, 2);</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <f t="shared" si="5"/>
+        <v>294</v>
+      </c>
+      <c r="B38" s="3">
+        <f>B37</f>
+        <v>73</v>
+      </c>
+      <c r="C38" s="3">
+        <v>61</v>
+      </c>
+      <c r="D38" s="3">
+        <v>4</v>
+      </c>
+      <c r="E38" s="3">
+        <v>0</v>
+      </c>
+      <c r="F38" s="3">
+        <v>1</v>
+      </c>
+      <c r="G38" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (294, 73, 61, 4, 0, 1);</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <f t="shared" si="5"/>
+        <v>295</v>
+      </c>
+      <c r="B39" s="3">
+        <f>B37</f>
+        <v>73</v>
+      </c>
+      <c r="C39" s="3">
+        <v>689</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0</v>
+      </c>
+      <c r="E39" s="3">
+        <v>0</v>
+      </c>
+      <c r="F39" s="3">
+        <v>2</v>
+      </c>
+      <c r="G39" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (295, 73, 689, 0, 0, 2);</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <f t="shared" si="5"/>
+        <v>296</v>
+      </c>
+      <c r="B40" s="3">
+        <f>B37</f>
+        <v>73</v>
+      </c>
+      <c r="C40" s="3">
+        <v>689</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0</v>
+      </c>
+      <c r="E40" s="3">
+        <v>0</v>
+      </c>
+      <c r="F40" s="3">
+        <v>1</v>
+      </c>
+      <c r="G40" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (296, 73, 689, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <f t="shared" si="5"/>
+        <v>297</v>
+      </c>
+      <c r="B41">
+        <f>B37+1</f>
+        <v>74</v>
+      </c>
+      <c r="C41" s="4">
+        <v>679</v>
+      </c>
+      <c r="D41" s="4">
+        <v>1</v>
+      </c>
+      <c r="E41" s="5">
+        <v>3</v>
+      </c>
+      <c r="F41" s="4">
+        <v>2</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (297, 74, 679, 1, 3, 2);</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <f t="shared" si="5"/>
+        <v>298</v>
+      </c>
+      <c r="B42">
+        <f>B41</f>
+        <v>74</v>
+      </c>
+      <c r="C42" s="4">
+        <v>679</v>
+      </c>
+      <c r="D42" s="4">
+        <v>0</v>
+      </c>
+      <c r="E42" s="5">
+        <v>0</v>
+      </c>
+      <c r="F42" s="4">
+        <v>1</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (298, 74, 679, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <f t="shared" si="5"/>
+        <v>299</v>
+      </c>
+      <c r="B43">
+        <f>B41</f>
+        <v>74</v>
+      </c>
+      <c r="C43" s="4">
+        <v>678</v>
+      </c>
+      <c r="D43" s="4">
+        <v>0</v>
+      </c>
+      <c r="E43" s="5">
+        <v>0</v>
+      </c>
+      <c r="F43" s="4">
+        <v>2</v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (299, 74, 678, 0, 0, 2);</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <f t="shared" si="5"/>
+        <v>300</v>
+      </c>
+      <c r="B44">
+        <f>B41</f>
+        <v>74</v>
+      </c>
+      <c r="C44" s="4">
+        <v>678</v>
+      </c>
+      <c r="D44" s="4">
+        <v>0</v>
+      </c>
+      <c r="E44" s="5">
+        <v>0</v>
+      </c>
+      <c r="F44" s="4">
+        <v>1</v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (300, 74, 678, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <f t="shared" si="5"/>
+        <v>301</v>
+      </c>
+      <c r="B45" s="3">
+        <f>B41+1</f>
+        <v>75</v>
+      </c>
+      <c r="C45" s="3">
+        <v>61</v>
+      </c>
+      <c r="D45" s="3">
+        <v>6</v>
+      </c>
+      <c r="E45" s="3">
+        <v>3</v>
+      </c>
+      <c r="F45" s="3">
+        <v>2</v>
+      </c>
+      <c r="G45" s="3" t="str">
+        <f t="shared" ref="G45:G88" si="6">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A45 &amp; ", " &amp; B45 &amp; ", " &amp; C45 &amp; ", " &amp; D45 &amp; ", " &amp; E45 &amp; ", " &amp; F45 &amp; ");"</f>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (301, 75, 61, 6, 3, 2);</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <f t="shared" si="5"/>
+        <v>302</v>
+      </c>
+      <c r="B46" s="3">
+        <f>B45</f>
+        <v>75</v>
+      </c>
+      <c r="C46" s="3">
+        <v>61</v>
+      </c>
+      <c r="D46" s="3">
+        <v>2</v>
+      </c>
+      <c r="E46" s="3">
+        <v>0</v>
+      </c>
+      <c r="F46" s="3">
+        <v>1</v>
+      </c>
+      <c r="G46" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (302, 75, 61, 2, 0, 1);</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <f t="shared" si="5"/>
+        <v>303</v>
+      </c>
+      <c r="B47" s="3">
+        <f>B45</f>
+        <v>75</v>
+      </c>
+      <c r="C47" s="3">
+        <v>679</v>
+      </c>
+      <c r="D47" s="3">
+        <v>1</v>
+      </c>
+      <c r="E47" s="3">
+        <v>0</v>
+      </c>
+      <c r="F47" s="3">
+        <v>2</v>
+      </c>
+      <c r="G47" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (303, 75, 679, 1, 0, 2);</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <f t="shared" si="5"/>
+        <v>304</v>
+      </c>
+      <c r="B48" s="3">
+        <f>B45</f>
+        <v>75</v>
+      </c>
+      <c r="C48" s="3">
+        <v>679</v>
+      </c>
+      <c r="D48" s="3">
+        <v>1</v>
+      </c>
+      <c r="E48" s="3">
+        <v>0</v>
+      </c>
+      <c r="F48" s="3">
+        <v>1</v>
+      </c>
+      <c r="G48" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (304, 75, 679, 1, 0, 1);</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <f t="shared" si="5"/>
+        <v>305</v>
+      </c>
+      <c r="B49">
+        <f>B45+1</f>
+        <v>76</v>
+      </c>
+      <c r="C49" s="4">
+        <v>689</v>
+      </c>
+      <c r="D49" s="4">
+        <v>0</v>
+      </c>
+      <c r="E49" s="5">
+        <v>0</v>
+      </c>
+      <c r="F49" s="4">
+        <v>2</v>
+      </c>
+      <c r="G49" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (305, 76, 689, 0, 0, 2);</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
+        <f t="shared" si="5"/>
+        <v>306</v>
+      </c>
+      <c r="B50">
+        <f>B49</f>
+        <v>76</v>
+      </c>
+      <c r="C50" s="4">
+        <v>689</v>
+      </c>
+      <c r="D50" s="4">
+        <v>0</v>
+      </c>
+      <c r="E50" s="5">
+        <v>0</v>
+      </c>
+      <c r="F50" s="4">
+        <v>1</v>
+      </c>
+      <c r="G50" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (306, 76, 689, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <f t="shared" si="5"/>
+        <v>307</v>
+      </c>
+      <c r="B51">
+        <f>B49</f>
+        <v>76</v>
+      </c>
+      <c r="C51" s="4">
+        <v>677</v>
+      </c>
+      <c r="D51" s="4">
+        <v>4</v>
+      </c>
+      <c r="E51" s="5">
+        <v>3</v>
+      </c>
+      <c r="F51" s="4">
+        <v>2</v>
+      </c>
+      <c r="G51" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (307, 76, 677, 4, 3, 2);</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <f t="shared" si="5"/>
+        <v>308</v>
+      </c>
+      <c r="B52">
+        <f>B49</f>
+        <v>76</v>
+      </c>
+      <c r="C52" s="4">
+        <v>677</v>
+      </c>
+      <c r="D52" s="4">
+        <v>3</v>
+      </c>
+      <c r="E52" s="5">
+        <v>0</v>
+      </c>
+      <c r="F52" s="4">
+        <v>1</v>
+      </c>
+      <c r="G52" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (308, 76, 677, 3, 0, 1);</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="3">
+        <f t="shared" si="5"/>
+        <v>309</v>
+      </c>
+      <c r="B53" s="3">
+        <f>B49+1</f>
+        <v>77</v>
+      </c>
+      <c r="C53" s="3">
+        <v>678</v>
+      </c>
+      <c r="D53" s="3">
+        <v>4</v>
+      </c>
+      <c r="E53" s="3">
+        <v>3</v>
+      </c>
+      <c r="F53" s="3">
+        <v>2</v>
+      </c>
+      <c r="G53" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (309, 77, 678, 4, 3, 2);</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="3">
+        <f t="shared" si="5"/>
+        <v>310</v>
+      </c>
+      <c r="B54" s="3">
+        <f>B53</f>
+        <v>77</v>
+      </c>
+      <c r="C54" s="3">
+        <v>678</v>
+      </c>
+      <c r="D54" s="3">
+        <v>1</v>
+      </c>
+      <c r="E54" s="3">
+        <v>0</v>
+      </c>
+      <c r="F54" s="3">
+        <v>1</v>
+      </c>
+      <c r="G54" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (310, 77, 678, 1, 0, 1);</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="3">
+        <f t="shared" si="5"/>
+        <v>311</v>
+      </c>
+      <c r="B55" s="3">
+        <f>B53</f>
+        <v>77</v>
+      </c>
+      <c r="C55" s="3">
+        <v>64</v>
+      </c>
+      <c r="D55" s="3">
+        <v>2</v>
+      </c>
+      <c r="E55" s="3">
+        <v>0</v>
+      </c>
+      <c r="F55" s="3">
+        <v>2</v>
+      </c>
+      <c r="G55" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (311, 77, 64, 2, 0, 2);</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
+        <f t="shared" si="5"/>
+        <v>312</v>
+      </c>
+      <c r="B56" s="3">
+        <f>B53</f>
+        <v>77</v>
+      </c>
+      <c r="C56" s="3">
+        <v>64</v>
+      </c>
+      <c r="D56" s="3">
+        <v>0</v>
+      </c>
+      <c r="E56" s="3">
+        <v>0</v>
+      </c>
+      <c r="F56" s="3">
+        <v>1</v>
+      </c>
+      <c r="G56" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (312, 77, 64, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
+        <f t="shared" si="5"/>
+        <v>313</v>
+      </c>
+      <c r="B57">
+        <f>B53+1</f>
+        <v>78</v>
+      </c>
+      <c r="C57" s="4">
+        <v>61</v>
+      </c>
+      <c r="D57" s="4">
+        <v>10</v>
+      </c>
+      <c r="E57" s="5">
+        <v>3</v>
+      </c>
+      <c r="F57" s="4">
+        <v>2</v>
+      </c>
+      <c r="G57" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (313, 78, 61, 10, 3, 2);</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="4">
+        <f t="shared" si="5"/>
+        <v>314</v>
+      </c>
+      <c r="B58">
+        <f>B57</f>
+        <v>78</v>
+      </c>
+      <c r="C58" s="4">
+        <v>61</v>
+      </c>
+      <c r="D58" s="4">
+        <v>5</v>
+      </c>
+      <c r="E58" s="5">
+        <v>0</v>
+      </c>
+      <c r="F58" s="4">
+        <v>1</v>
+      </c>
+      <c r="G58" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (314, 78, 61, 5, 0, 1);</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
+        <f t="shared" si="5"/>
+        <v>315</v>
+      </c>
+      <c r="B59">
+        <f>B57</f>
+        <v>78</v>
+      </c>
+      <c r="C59" s="4">
+        <v>689</v>
+      </c>
+      <c r="D59" s="4">
+        <v>0</v>
+      </c>
+      <c r="E59" s="5">
+        <v>0</v>
+      </c>
+      <c r="F59" s="4">
+        <v>2</v>
+      </c>
+      <c r="G59" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (315, 78, 689, 0, 0, 2);</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="4">
+        <f t="shared" si="5"/>
+        <v>316</v>
+      </c>
+      <c r="B60">
+        <f>B57</f>
+        <v>78</v>
+      </c>
+      <c r="C60" s="4">
+        <v>689</v>
+      </c>
+      <c r="D60" s="4">
+        <v>0</v>
+      </c>
+      <c r="E60" s="5">
+        <v>0</v>
+      </c>
+      <c r="F60" s="4">
+        <v>1</v>
+      </c>
+      <c r="G60" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (316, 78, 689, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="3">
+        <f t="shared" si="5"/>
+        <v>317</v>
+      </c>
+      <c r="B61" s="3">
+        <f>B57+1</f>
+        <v>79</v>
+      </c>
+      <c r="C61" s="3">
+        <v>679</v>
+      </c>
+      <c r="D61" s="3">
+        <v>1</v>
+      </c>
+      <c r="E61" s="3">
+        <v>0</v>
+      </c>
+      <c r="F61" s="3">
+        <v>2</v>
+      </c>
+      <c r="G61" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (317, 79, 679, 1, 0, 2);</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="3">
+        <f t="shared" si="5"/>
+        <v>318</v>
+      </c>
+      <c r="B62" s="3">
+        <f>B61</f>
+        <v>79</v>
+      </c>
+      <c r="C62" s="3">
+        <v>679</v>
+      </c>
+      <c r="D62" s="3">
+        <v>1</v>
+      </c>
+      <c r="E62" s="3">
+        <v>0</v>
+      </c>
+      <c r="F62" s="3">
+        <v>1</v>
+      </c>
+      <c r="G62" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (318, 79, 679, 1, 0, 1);</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="3">
+        <f t="shared" si="5"/>
+        <v>319</v>
+      </c>
+      <c r="B63" s="3">
+        <f>B61</f>
+        <v>79</v>
+      </c>
+      <c r="C63" s="3">
+        <v>677</v>
+      </c>
+      <c r="D63" s="3">
+        <v>2</v>
+      </c>
+      <c r="E63" s="3">
+        <v>3</v>
+      </c>
+      <c r="F63" s="3">
+        <v>2</v>
+      </c>
+      <c r="G63" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (319, 79, 677, 2, 3, 2);</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="3">
+        <f t="shared" si="5"/>
+        <v>320</v>
+      </c>
+      <c r="B64" s="3">
+        <f>B61</f>
+        <v>79</v>
+      </c>
+      <c r="C64" s="3">
+        <v>677</v>
+      </c>
+      <c r="D64" s="3">
+        <v>1</v>
+      </c>
+      <c r="E64" s="3">
+        <v>0</v>
+      </c>
+      <c r="F64" s="3">
+        <v>1</v>
+      </c>
+      <c r="G64" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (320, 79, 677, 1, 0, 1);</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="4">
+        <f t="shared" si="5"/>
+        <v>321</v>
+      </c>
+      <c r="B65">
+        <f>B61+1</f>
+        <v>80</v>
+      </c>
+      <c r="C65" s="4">
+        <v>678</v>
+      </c>
+      <c r="D65" s="4">
+        <v>0</v>
+      </c>
+      <c r="E65" s="5">
+        <v>0</v>
+      </c>
+      <c r="F65" s="4">
+        <v>2</v>
+      </c>
+      <c r="G65" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (321, 80, 678, 0, 0, 2);</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="4">
+        <f t="shared" si="5"/>
+        <v>322</v>
+      </c>
+      <c r="B66">
+        <f>B65</f>
+        <v>80</v>
+      </c>
+      <c r="C66" s="4">
+        <v>678</v>
+      </c>
+      <c r="D66" s="4">
+        <v>0</v>
+      </c>
+      <c r="E66" s="5">
+        <v>0</v>
+      </c>
+      <c r="F66" s="4">
+        <v>1</v>
+      </c>
+      <c r="G66" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (322, 80, 678, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="4">
+        <f t="shared" si="5"/>
+        <v>323</v>
+      </c>
+      <c r="B67">
+        <f>B65</f>
+        <v>80</v>
+      </c>
+      <c r="C67" s="4">
+        <v>61</v>
+      </c>
+      <c r="D67" s="4">
+        <v>3</v>
+      </c>
+      <c r="E67" s="5">
+        <v>3</v>
+      </c>
+      <c r="F67" s="4">
+        <v>2</v>
+      </c>
+      <c r="G67" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (323, 80, 61, 3, 3, 2);</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="4">
+        <f t="shared" si="5"/>
+        <v>324</v>
+      </c>
+      <c r="B68">
+        <f>B65</f>
+        <v>80</v>
+      </c>
+      <c r="C68" s="4">
+        <v>61</v>
+      </c>
+      <c r="D68" s="4">
+        <v>1</v>
+      </c>
+      <c r="E68" s="5">
+        <v>0</v>
+      </c>
+      <c r="F68" s="4">
+        <v>1</v>
+      </c>
+      <c r="G68" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (324, 80, 61, 1, 0, 1);</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="3">
+        <f t="shared" si="5"/>
+        <v>325</v>
+      </c>
+      <c r="B69" s="3">
+        <f>B65+1</f>
+        <v>81</v>
+      </c>
+      <c r="C69" s="3">
+        <v>689</v>
+      </c>
+      <c r="D69" s="3">
+        <v>2</v>
+      </c>
+      <c r="E69" s="3">
+        <v>3</v>
+      </c>
+      <c r="F69" s="3">
+        <v>2</v>
+      </c>
+      <c r="G69" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (325, 81, 689, 2, 3, 2);</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="3">
+        <f t="shared" si="5"/>
+        <v>326</v>
+      </c>
+      <c r="B70" s="3">
+        <f>B69</f>
+        <v>81</v>
+      </c>
+      <c r="C70" s="3">
+        <v>689</v>
+      </c>
+      <c r="D70" s="3">
+        <v>1</v>
+      </c>
+      <c r="E70" s="3">
+        <v>0</v>
+      </c>
+      <c r="F70" s="3">
+        <v>1</v>
+      </c>
+      <c r="G70" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (326, 81, 689, 1, 0, 1);</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="3">
+        <f t="shared" si="5"/>
+        <v>327</v>
+      </c>
+      <c r="B71" s="3">
+        <f>B69</f>
+        <v>81</v>
+      </c>
+      <c r="C71" s="3">
+        <v>678</v>
+      </c>
+      <c r="D71" s="3">
+        <v>1</v>
+      </c>
+      <c r="E71" s="3">
+        <v>0</v>
+      </c>
+      <c r="F71" s="3">
+        <v>2</v>
+      </c>
+      <c r="G71" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (327, 81, 678, 1, 0, 2);</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="3">
+        <f t="shared" si="5"/>
+        <v>328</v>
+      </c>
+      <c r="B72" s="3">
+        <f>B69</f>
+        <v>81</v>
+      </c>
+      <c r="C72" s="3">
+        <v>678</v>
+      </c>
+      <c r="D72" s="3">
+        <v>1</v>
+      </c>
+      <c r="E72" s="3">
+        <v>0</v>
+      </c>
+      <c r="F72" s="3">
+        <v>1</v>
+      </c>
+      <c r="G72" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (328, 81, 678, 1, 0, 1);</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="4">
+        <f t="shared" si="5"/>
+        <v>329</v>
+      </c>
+      <c r="B73">
+        <f>B69+1</f>
+        <v>82</v>
+      </c>
+      <c r="C73" s="4">
+        <v>679</v>
+      </c>
+      <c r="D73" s="4">
+        <v>0</v>
+      </c>
+      <c r="E73" s="5">
+        <v>0</v>
+      </c>
+      <c r="F73" s="4">
+        <v>2</v>
+      </c>
+      <c r="G73" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (329, 82, 679, 0, 0, 2);</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="4">
+        <f t="shared" si="5"/>
+        <v>330</v>
+      </c>
+      <c r="B74">
+        <f>B73</f>
+        <v>82</v>
+      </c>
+      <c r="C74" s="4">
+        <v>679</v>
+      </c>
+      <c r="D74" s="4">
+        <v>0</v>
+      </c>
+      <c r="E74" s="5">
+        <v>0</v>
+      </c>
+      <c r="F74" s="4">
+        <v>1</v>
+      </c>
+      <c r="G74" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (330, 82, 679, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="4">
+        <f t="shared" si="5"/>
+        <v>331</v>
+      </c>
+      <c r="B75">
+        <f>B73</f>
+        <v>82</v>
+      </c>
+      <c r="C75" s="4">
+        <v>64</v>
+      </c>
+      <c r="D75" s="4">
+        <v>2</v>
+      </c>
+      <c r="E75" s="5">
+        <v>3</v>
+      </c>
+      <c r="F75" s="4">
+        <v>2</v>
+      </c>
+      <c r="G75" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (331, 82, 64, 2, 3, 2);</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="4">
+        <f t="shared" si="5"/>
+        <v>332</v>
+      </c>
+      <c r="B76">
+        <f>B73</f>
+        <v>82</v>
+      </c>
+      <c r="C76" s="4">
+        <v>64</v>
+      </c>
+      <c r="D76" s="4">
+        <v>1</v>
+      </c>
+      <c r="E76" s="5">
+        <v>0</v>
+      </c>
+      <c r="F76" s="4">
+        <v>1</v>
+      </c>
+      <c r="G76" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (332, 82, 64, 1, 0, 1);</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="3">
+        <f t="shared" si="5"/>
+        <v>333</v>
+      </c>
+      <c r="B77" s="3">
+        <f>B73+1</f>
+        <v>83</v>
+      </c>
+      <c r="C77" s="3">
+        <v>677</v>
+      </c>
+      <c r="D77" s="3">
+        <v>2</v>
+      </c>
+      <c r="E77" s="3">
+        <v>1</v>
+      </c>
+      <c r="F77" s="3">
+        <v>2</v>
+      </c>
+      <c r="G77" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (333, 83, 677, 2, 1, 2);</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="3">
+        <f t="shared" si="5"/>
+        <v>334</v>
+      </c>
+      <c r="B78" s="3">
+        <f>B77</f>
+        <v>83</v>
+      </c>
+      <c r="C78" s="3">
+        <v>677</v>
+      </c>
+      <c r="D78" s="3">
+        <v>1</v>
+      </c>
+      <c r="E78" s="3">
+        <v>0</v>
+      </c>
+      <c r="F78" s="3">
+        <v>1</v>
+      </c>
+      <c r="G78" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (334, 83, 677, 1, 0, 1);</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="3">
+        <f t="shared" si="5"/>
+        <v>335</v>
+      </c>
+      <c r="B79" s="3">
+        <f>B77</f>
+        <v>83</v>
+      </c>
+      <c r="C79" s="3">
+        <v>61</v>
+      </c>
+      <c r="D79" s="3">
+        <v>2</v>
+      </c>
+      <c r="E79" s="3">
+        <v>1</v>
+      </c>
+      <c r="F79" s="3">
+        <v>2</v>
+      </c>
+      <c r="G79" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (335, 83, 61, 2, 1, 2);</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="3">
+        <f t="shared" si="5"/>
+        <v>336</v>
+      </c>
+      <c r="B80" s="3">
+        <f>B77</f>
+        <v>83</v>
+      </c>
+      <c r="C80" s="3">
+        <v>61</v>
+      </c>
+      <c r="D80" s="3">
+        <v>0</v>
+      </c>
+      <c r="E80" s="3">
+        <v>0</v>
+      </c>
+      <c r="F80" s="3">
+        <v>1</v>
+      </c>
+      <c r="G80" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (336, 83, 61, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="4">
+        <f t="shared" si="5"/>
+        <v>337</v>
+      </c>
+      <c r="B81">
+        <f>B77+1</f>
+        <v>84</v>
+      </c>
+      <c r="C81" s="4">
+        <v>677</v>
+      </c>
+      <c r="D81" s="4">
+        <v>1</v>
+      </c>
+      <c r="E81" s="5">
+        <v>0</v>
+      </c>
+      <c r="F81" s="4">
+        <v>2</v>
+      </c>
+      <c r="G81" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (337, 84, 677, 1, 0, 2);</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="4">
+        <f t="shared" si="5"/>
+        <v>338</v>
+      </c>
+      <c r="B82">
+        <f>B81</f>
+        <v>84</v>
+      </c>
+      <c r="C82" s="4">
+        <v>677</v>
+      </c>
+      <c r="D82" s="4">
+        <v>0</v>
+      </c>
+      <c r="E82" s="5">
+        <v>0</v>
+      </c>
+      <c r="F82" s="4">
+        <v>1</v>
+      </c>
+      <c r="G82" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (338, 84, 677, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="4">
+        <f t="shared" si="5"/>
+        <v>339</v>
+      </c>
+      <c r="B83">
+        <f>B81</f>
+        <v>84</v>
+      </c>
+      <c r="C83" s="4">
+        <v>61</v>
+      </c>
+      <c r="D83" s="4">
+        <v>5</v>
+      </c>
+      <c r="E83" s="5">
+        <v>3</v>
+      </c>
+      <c r="F83" s="4">
+        <v>2</v>
+      </c>
+      <c r="G83" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (339, 84, 61, 5, 3, 2);</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="4">
+        <f t="shared" si="5"/>
+        <v>340</v>
+      </c>
+      <c r="B84">
+        <f>B81</f>
+        <v>84</v>
+      </c>
+      <c r="C84" s="4">
+        <v>61</v>
+      </c>
+      <c r="D84" s="4">
+        <v>4</v>
+      </c>
+      <c r="E84" s="5">
+        <v>0</v>
+      </c>
+      <c r="F84" s="4">
+        <v>1</v>
+      </c>
+      <c r="G84" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (340, 84, 61, 4, 0, 1);</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="3">
+        <f t="shared" si="5"/>
+        <v>341</v>
+      </c>
+      <c r="B85" s="3">
+        <f>B81+1</f>
+        <v>85</v>
+      </c>
+      <c r="C85" s="3">
+        <v>61</v>
+      </c>
+      <c r="D85" s="3">
+        <v>6</v>
+      </c>
+      <c r="E85" s="3">
+        <v>3</v>
+      </c>
+      <c r="F85" s="3">
+        <v>2</v>
+      </c>
+      <c r="G85" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (341, 85, 61, 6, 3, 2);</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="3">
+        <f t="shared" si="5"/>
+        <v>342</v>
+      </c>
+      <c r="B86" s="3">
+        <f>B85</f>
+        <v>85</v>
+      </c>
+      <c r="C86" s="3">
+        <v>61</v>
+      </c>
+      <c r="D86" s="3">
+        <v>2</v>
+      </c>
+      <c r="E86" s="3">
+        <v>0</v>
+      </c>
+      <c r="F86" s="3">
+        <v>1</v>
+      </c>
+      <c r="G86" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (342, 85, 61, 2, 0, 1);</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="3">
+        <f t="shared" si="5"/>
+        <v>343</v>
+      </c>
+      <c r="B87" s="3">
+        <f>B85</f>
+        <v>85</v>
+      </c>
+      <c r="C87" s="3">
+        <v>677</v>
+      </c>
+      <c r="D87" s="3">
+        <v>0</v>
+      </c>
+      <c r="E87" s="3">
+        <v>0</v>
+      </c>
+      <c r="F87" s="3">
+        <v>2</v>
+      </c>
+      <c r="G87" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (343, 85, 677, 0, 0, 2);</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="3">
+        <f t="shared" si="5"/>
+        <v>344</v>
+      </c>
+      <c r="B88" s="3">
+        <f>B85</f>
+        <v>85</v>
+      </c>
+      <c r="C88" s="3">
+        <v>677</v>
+      </c>
+      <c r="D88" s="3">
+        <v>0</v>
+      </c>
+      <c r="E88" s="3">
+        <v>0</v>
+      </c>
+      <c r="F88" s="3">
+        <v>1</v>
+      </c>
+      <c r="G88" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (344, 85, 677, 0, 0, 1);</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="111.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="str">
+        <f>"insert into game (matchid, matchdate, game_type, country) values (" &amp; A1 &amp; ", '" &amp; B1 &amp; "', " &amp; C1 &amp; ", " &amp; D1 &amp;  ");"</f>
+        <v>insert into game (matchid, matchdate, game_type, country) values (matchid, 'matchdate', game_type, country);</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <f>'2004'!A18 + 1</f>
+        <v>86</v>
+      </c>
+      <c r="B2" s="2" t="str">
+        <f>"2007-10-17"</f>
+        <v>2007-10-17</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>679</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G13" si="0">"insert into game (matchid, matchdate, game_type, country) values (" &amp; A2 &amp; ", '" &amp; B2 &amp; "', " &amp; C2 &amp; ", " &amp; D2 &amp;  ");"</f>
+        <v>insert into game (matchid, matchdate, game_type, country) values (86, '2007-10-17', 2, 679);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>87</v>
+      </c>
+      <c r="B3" s="2" t="str">
+        <f>"2007-11-17"</f>
+        <v>2007-11-17</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>678</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (87, '2007-11-17', 2, 678);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A13" si="1">A3+1</f>
+        <v>88</v>
+      </c>
+      <c r="B4" s="2" t="str">
+        <f>"2007-11-17"</f>
+        <v>2007-11-17</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>679</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (88, '2007-11-17', 2, 679);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="B5" s="2" t="str">
+        <f>"2007-11-21"</f>
+        <v>2007-11-21</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>64</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (89, '2007-11-21', 2, 64);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="B6" s="2" t="str">
+        <f>"2007-11-21"</f>
+        <v>2007-11-21</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>687</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (90, '2007-11-21', 2, 687);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="B7" s="2" t="str">
+        <f>"2008-07-14"</f>
+        <v>2008-07-14</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>678</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (91, '2008-07-14', 2, 678);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="B8" s="2" t="str">
+        <f>"2008-07-21"</f>
+        <v>2008-07-21</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>687</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (92, '2008-07-21', 2, 687);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="B9" s="2" t="str">
+        <f>"2008-09-06"</f>
+        <v>2008-09-06</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>679</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (93, '2008-09-06', 2, 679);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="B10" s="2" t="str">
+        <f>"2008-09-06"</f>
+        <v>2008-09-06</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>687</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (94, '2008-09-06', 2, 687);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="B11" s="2" t="str">
+        <f>"2008-09-10"</f>
+        <v>2008-09-10</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>678</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (95, '2008-09-10', 2, 678);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="B12" s="2" t="str">
+        <f>"2008-09-10"</f>
+        <v>2008-09-10</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>64</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (96, '2008-09-10', 2, 64);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="B13" s="2" t="str">
+        <f>"2008-11-19"</f>
+        <v>2008-11-19</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>679</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (97, '2008-11-19', 2, 679);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" t="str">
+        <f>"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A15 &amp; ", " &amp; B15 &amp; ", " &amp; C15 &amp; ", " &amp; D15 &amp; ", " &amp; E15 &amp; ", " &amp; F15 &amp; ");"</f>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (id, matchid, squad, goals, points, time_type);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <f>'2004'!A88 + 1</f>
+        <v>345</v>
+      </c>
+      <c r="B16" s="3">
+        <f>A2</f>
+        <v>86</v>
+      </c>
+      <c r="C16" s="3">
+        <v>679</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <v>2</v>
+      </c>
+      <c r="G16" s="3" t="str">
+        <f t="shared" ref="G16:G63" si="2">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A16 &amp; ", " &amp; B16 &amp; ", " &amp; C16 &amp; ", " &amp; D16 &amp; ", " &amp; E16 &amp; ", " &amp; F16 &amp; ");"</f>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (345, 86, 679, 0, 0, 2);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <f>A16+1</f>
+        <v>346</v>
+      </c>
+      <c r="B17" s="3">
+        <f>B16</f>
+        <v>86</v>
+      </c>
+      <c r="C17" s="3">
+        <v>679</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1</v>
+      </c>
+      <c r="G17" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (346, 86, 679, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <f t="shared" ref="A18:A23" si="3">A17+1</f>
+        <v>347</v>
+      </c>
+      <c r="B18" s="3">
+        <f>B16</f>
+        <v>86</v>
+      </c>
+      <c r="C18" s="3">
+        <v>64</v>
+      </c>
+      <c r="D18" s="3">
+        <v>2</v>
+      </c>
+      <c r="E18" s="3">
+        <v>3</v>
+      </c>
+      <c r="F18" s="3">
+        <v>2</v>
+      </c>
+      <c r="G18" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (347, 86, 64, 2, 3, 2);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <f t="shared" si="3"/>
+        <v>348</v>
+      </c>
+      <c r="B19" s="3">
+        <f>B16</f>
+        <v>86</v>
+      </c>
+      <c r="C19" s="3">
+        <v>64</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
+      <c r="G19" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (348, 86, 64, 1, 0, 1);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="3"/>
+        <v>349</v>
+      </c>
+      <c r="B20">
+        <f>B16+1</f>
+        <v>87</v>
+      </c>
+      <c r="C20" s="4">
+        <v>678</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0</v>
+      </c>
+      <c r="F20" s="4">
+        <v>2</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (349, 87, 678, 1, 0, 2);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="3"/>
+        <v>350</v>
+      </c>
+      <c r="B21">
+        <f>B20</f>
+        <v>87</v>
+      </c>
+      <c r="C21" s="4">
+        <v>678</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0</v>
+      </c>
+      <c r="F21" s="4">
+        <v>1</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (350, 87, 678, 1, 0, 1);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="3"/>
+        <v>351</v>
+      </c>
+      <c r="B22">
+        <f>B20</f>
+        <v>87</v>
+      </c>
+      <c r="C22" s="4">
+        <v>64</v>
+      </c>
+      <c r="D22" s="4">
+        <v>2</v>
+      </c>
+      <c r="E22" s="5">
+        <v>3</v>
+      </c>
+      <c r="F22" s="4">
+        <v>2</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (351, 87, 64, 2, 3, 2);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="3"/>
+        <v>352</v>
+      </c>
+      <c r="B23">
+        <f>B20</f>
+        <v>87</v>
+      </c>
+      <c r="C23" s="4">
+        <v>64</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0</v>
+      </c>
+      <c r="F23" s="4">
+        <v>1</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (352, 87, 64, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <f>A23+1</f>
+        <v>353</v>
+      </c>
+      <c r="B24" s="3">
+        <f>B20+1</f>
+        <v>88</v>
+      </c>
+      <c r="C24" s="3">
+        <v>679</v>
+      </c>
+      <c r="D24" s="3">
+        <v>3</v>
+      </c>
+      <c r="E24" s="3">
+        <v>1</v>
+      </c>
+      <c r="F24" s="3">
+        <v>2</v>
+      </c>
+      <c r="G24" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (353, 88, 679, 3, 1, 2);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <f>A24+1</f>
+        <v>354</v>
+      </c>
+      <c r="B25" s="3">
+        <f>B24</f>
+        <v>88</v>
+      </c>
+      <c r="C25" s="3">
+        <v>679</v>
+      </c>
+      <c r="D25" s="3">
+        <v>2</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3">
+        <v>1</v>
+      </c>
+      <c r="G25" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (354, 88, 679, 2, 0, 1);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <f>A25+1</f>
+        <v>355</v>
+      </c>
+      <c r="B26" s="3">
+        <f>B24</f>
+        <v>88</v>
+      </c>
+      <c r="C26" s="3">
+        <v>687</v>
+      </c>
+      <c r="D26" s="3">
+        <v>3</v>
+      </c>
+      <c r="E26" s="3">
+        <v>1</v>
+      </c>
+      <c r="F26" s="3">
+        <v>2</v>
+      </c>
+      <c r="G26" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (355, 88, 687, 3, 1, 2);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <f>A26+1</f>
+        <v>356</v>
+      </c>
+      <c r="B27" s="3">
+        <f>B24</f>
+        <v>88</v>
+      </c>
+      <c r="C27" s="3">
+        <v>687</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0</v>
+      </c>
+      <c r="F27" s="3">
+        <v>1</v>
+      </c>
+      <c r="G27" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (356, 88, 687, 1, 0, 1);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <f>A27+1</f>
+        <v>357</v>
+      </c>
+      <c r="B28">
+        <f>B24+1</f>
+        <v>89</v>
+      </c>
+      <c r="C28" s="4">
+        <v>64</v>
+      </c>
+      <c r="D28" s="4">
+        <v>4</v>
+      </c>
+      <c r="E28" s="5">
+        <v>3</v>
+      </c>
+      <c r="F28" s="4">
+        <v>2</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (357, 89, 64, 4, 3, 2);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <f t="shared" ref="A29:A63" si="4">A28+1</f>
+        <v>358</v>
+      </c>
+      <c r="B29">
+        <f>B28</f>
+        <v>89</v>
+      </c>
+      <c r="C29" s="4">
+        <v>64</v>
+      </c>
+      <c r="D29" s="4">
+        <v>3</v>
+      </c>
+      <c r="E29" s="5">
+        <v>0</v>
+      </c>
+      <c r="F29" s="4">
+        <v>1</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (358, 89, 64, 3, 0, 1);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <f t="shared" si="4"/>
+        <v>359</v>
+      </c>
+      <c r="B30">
+        <f>B28</f>
+        <v>89</v>
+      </c>
+      <c r="C30" s="4">
+        <v>678</v>
+      </c>
+      <c r="D30" s="4">
+        <v>1</v>
+      </c>
+      <c r="E30" s="5">
+        <v>0</v>
+      </c>
+      <c r="F30" s="4">
+        <v>2</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (359, 89, 678, 1, 0, 2);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <f t="shared" si="4"/>
+        <v>360</v>
+      </c>
+      <c r="B31">
+        <f>B28</f>
+        <v>89</v>
+      </c>
+      <c r="C31" s="4">
+        <v>678</v>
+      </c>
+      <c r="D31" s="4">
+        <v>0</v>
+      </c>
+      <c r="E31" s="5">
+        <v>0</v>
+      </c>
+      <c r="F31" s="4">
+        <v>1</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (360, 89, 678, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <f t="shared" si="4"/>
+        <v>361</v>
+      </c>
+      <c r="B32" s="3">
+        <f>B28+1</f>
+        <v>90</v>
+      </c>
+      <c r="C32" s="3">
+        <v>687</v>
+      </c>
+      <c r="D32" s="3">
+        <v>4</v>
+      </c>
+      <c r="E32" s="3">
+        <v>3</v>
+      </c>
+      <c r="F32" s="3">
+        <v>2</v>
+      </c>
+      <c r="G32" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (361, 90, 687, 4, 3, 2);</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <f t="shared" si="4"/>
+        <v>362</v>
+      </c>
+      <c r="B33" s="3">
+        <f>B32</f>
+        <v>90</v>
+      </c>
+      <c r="C33" s="3">
+        <v>687</v>
+      </c>
+      <c r="D33" s="3">
+        <v>2</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0</v>
+      </c>
+      <c r="F33" s="3">
+        <v>1</v>
+      </c>
+      <c r="G33" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (362, 90, 687, 2, 0, 1);</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <f t="shared" si="4"/>
+        <v>363</v>
+      </c>
+      <c r="B34" s="3">
+        <f>B32</f>
+        <v>90</v>
+      </c>
+      <c r="C34" s="3">
+        <v>679</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0</v>
+      </c>
+      <c r="E34" s="3">
+        <v>0</v>
+      </c>
+      <c r="F34" s="3">
+        <v>2</v>
+      </c>
+      <c r="G34" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (363, 90, 679, 0, 0, 2);</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <f t="shared" si="4"/>
+        <v>364</v>
+      </c>
+      <c r="B35" s="3">
+        <f>B32</f>
+        <v>90</v>
+      </c>
+      <c r="C35" s="3">
+        <v>679</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0</v>
+      </c>
+      <c r="E35" s="3">
+        <v>0</v>
+      </c>
+      <c r="F35" s="3">
+        <v>1</v>
+      </c>
+      <c r="G35" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (364, 90, 679, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <f t="shared" si="4"/>
+        <v>365</v>
+      </c>
+      <c r="B36">
+        <f>B32+1</f>
+        <v>91</v>
+      </c>
+      <c r="C36" s="4">
+        <v>678</v>
+      </c>
+      <c r="D36" s="4">
+        <v>1</v>
+      </c>
+      <c r="E36" s="5">
+        <v>1</v>
+      </c>
+      <c r="F36" s="4">
+        <v>2</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (365, 91, 678, 1, 1, 2);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <f t="shared" si="4"/>
+        <v>366</v>
+      </c>
+      <c r="B37">
+        <f>B36</f>
+        <v>91</v>
+      </c>
+      <c r="C37" s="4">
+        <v>678</v>
+      </c>
+      <c r="D37" s="4">
+        <v>0</v>
+      </c>
+      <c r="E37" s="5">
+        <v>0</v>
+      </c>
+      <c r="F37" s="4">
+        <v>1</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (366, 91, 678, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <f t="shared" si="4"/>
+        <v>367</v>
+      </c>
+      <c r="B38">
+        <f>B36</f>
+        <v>91</v>
+      </c>
+      <c r="C38" s="4">
+        <v>687</v>
+      </c>
+      <c r="D38" s="4">
+        <v>1</v>
+      </c>
+      <c r="E38" s="5">
+        <v>1</v>
+      </c>
+      <c r="F38" s="4">
+        <v>2</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (367, 91, 687, 1, 1, 2);</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <f t="shared" si="4"/>
+        <v>368</v>
+      </c>
+      <c r="B39">
+        <f>B36</f>
+        <v>91</v>
+      </c>
+      <c r="C39" s="4">
+        <v>687</v>
+      </c>
+      <c r="D39" s="4">
+        <v>0</v>
+      </c>
+      <c r="E39" s="5">
+        <v>0</v>
+      </c>
+      <c r="F39" s="4">
+        <v>1</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (368, 91, 687, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <f t="shared" si="4"/>
+        <v>369</v>
+      </c>
+      <c r="B40" s="3">
+        <f>B36+1</f>
+        <v>92</v>
+      </c>
+      <c r="C40" s="3">
+        <v>687</v>
+      </c>
+      <c r="D40" s="3">
+        <v>3</v>
+      </c>
+      <c r="E40" s="3">
+        <v>3</v>
+      </c>
+      <c r="F40" s="3">
+        <v>2</v>
+      </c>
+      <c r="G40" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (369, 92, 687, 3, 3, 2);</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <f t="shared" si="4"/>
+        <v>370</v>
+      </c>
+      <c r="B41" s="3">
+        <f>B40</f>
+        <v>92</v>
+      </c>
+      <c r="C41" s="3">
+        <v>687</v>
+      </c>
+      <c r="D41" s="3">
+        <v>1</v>
+      </c>
+      <c r="E41" s="3">
+        <v>0</v>
+      </c>
+      <c r="F41" s="3">
+        <v>1</v>
+      </c>
+      <c r="G41" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (370, 92, 687, 1, 0, 1);</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <f t="shared" si="4"/>
+        <v>371</v>
+      </c>
+      <c r="B42" s="3">
+        <f>B40</f>
+        <v>92</v>
+      </c>
+      <c r="C42" s="3">
+        <v>678</v>
+      </c>
+      <c r="D42" s="3">
+        <v>0</v>
+      </c>
+      <c r="E42" s="3">
+        <v>0</v>
+      </c>
+      <c r="F42" s="3">
+        <v>2</v>
+      </c>
+      <c r="G42" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (371, 92, 678, 0, 0, 2);</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <f t="shared" si="4"/>
+        <v>372</v>
+      </c>
+      <c r="B43" s="3">
+        <f>B40</f>
+        <v>92</v>
+      </c>
+      <c r="C43" s="3">
+        <v>678</v>
+      </c>
+      <c r="D43" s="3">
+        <v>0</v>
+      </c>
+      <c r="E43" s="3">
+        <v>0</v>
+      </c>
+      <c r="F43" s="3">
+        <v>1</v>
+      </c>
+      <c r="G43" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (372, 92, 678, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <f t="shared" si="4"/>
+        <v>373</v>
+      </c>
+      <c r="B44">
+        <f>B40+1</f>
+        <v>93</v>
+      </c>
+      <c r="C44" s="4">
+        <v>679</v>
+      </c>
+      <c r="D44" s="4">
+        <v>2</v>
+      </c>
+      <c r="E44" s="5">
+        <v>3</v>
+      </c>
+      <c r="F44" s="4">
+        <v>2</v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (373, 93, 679, 2, 3, 2);</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <f t="shared" si="4"/>
+        <v>374</v>
+      </c>
+      <c r="B45">
+        <f>B44</f>
+        <v>93</v>
+      </c>
+      <c r="C45" s="4">
+        <v>679</v>
+      </c>
+      <c r="D45" s="4">
+        <v>1</v>
+      </c>
+      <c r="E45" s="5">
+        <v>0</v>
+      </c>
+      <c r="F45" s="4">
+        <v>1</v>
+      </c>
+      <c r="G45" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (374, 93, 679, 1, 0, 1);</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <f t="shared" si="4"/>
+        <v>375</v>
+      </c>
+      <c r="B46">
+        <f>B44</f>
+        <v>93</v>
+      </c>
+      <c r="C46" s="4">
+        <v>678</v>
+      </c>
+      <c r="D46" s="4">
+        <v>0</v>
+      </c>
+      <c r="E46" s="5">
+        <v>0</v>
+      </c>
+      <c r="F46" s="4">
+        <v>2</v>
+      </c>
+      <c r="G46" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (375, 93, 678, 0, 0, 2);</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <f t="shared" si="4"/>
+        <v>376</v>
+      </c>
+      <c r="B47">
+        <f>B44</f>
+        <v>93</v>
+      </c>
+      <c r="C47" s="4">
+        <v>678</v>
+      </c>
+      <c r="D47" s="4">
+        <v>0</v>
+      </c>
+      <c r="E47" s="5">
+        <v>0</v>
+      </c>
+      <c r="F47" s="4">
+        <v>1</v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (376, 93, 678, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <f t="shared" si="4"/>
+        <v>377</v>
+      </c>
+      <c r="B48" s="3">
+        <f>B44+1</f>
+        <v>94</v>
+      </c>
+      <c r="C48" s="3">
+        <v>687</v>
+      </c>
+      <c r="D48" s="3">
+        <v>1</v>
+      </c>
+      <c r="E48" s="3">
+        <v>0</v>
+      </c>
+      <c r="F48" s="3">
+        <v>2</v>
+      </c>
+      <c r="G48" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (377, 94, 687, 1, 0, 2);</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <f t="shared" si="4"/>
+        <v>378</v>
+      </c>
+      <c r="B49" s="3">
+        <f>B48</f>
+        <v>94</v>
+      </c>
+      <c r="C49" s="3">
+        <v>687</v>
+      </c>
+      <c r="D49" s="3">
+        <v>0</v>
+      </c>
+      <c r="E49" s="3">
+        <v>0</v>
+      </c>
+      <c r="F49" s="3">
+        <v>1</v>
+      </c>
+      <c r="G49" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (378, 94, 687, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <f t="shared" si="4"/>
+        <v>379</v>
+      </c>
+      <c r="B50" s="3">
+        <f>B48</f>
+        <v>94</v>
+      </c>
+      <c r="C50" s="3">
+        <v>64</v>
+      </c>
+      <c r="D50" s="3">
+        <v>3</v>
+      </c>
+      <c r="E50" s="3">
+        <v>3</v>
+      </c>
+      <c r="F50" s="3">
+        <v>2</v>
+      </c>
+      <c r="G50" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (379, 94, 64, 3, 3, 2);</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <f t="shared" si="4"/>
+        <v>380</v>
+      </c>
+      <c r="B51" s="3">
+        <f>B48</f>
+        <v>94</v>
+      </c>
+      <c r="C51" s="3">
+        <v>64</v>
+      </c>
+      <c r="D51" s="3">
+        <v>1</v>
+      </c>
+      <c r="E51" s="3">
+        <v>0</v>
+      </c>
+      <c r="F51" s="3">
+        <v>1</v>
+      </c>
+      <c r="G51" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (380, 94, 64, 1, 0, 1);</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <f t="shared" si="4"/>
+        <v>381</v>
+      </c>
+      <c r="B52">
+        <f>B48+1</f>
+        <v>95</v>
+      </c>
+      <c r="C52" s="4">
+        <v>678</v>
+      </c>
+      <c r="D52" s="4">
+        <v>2</v>
+      </c>
+      <c r="E52" s="5">
+        <v>3</v>
+      </c>
+      <c r="F52" s="4">
+        <v>2</v>
+      </c>
+      <c r="G52" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (381, 95, 678, 2, 3, 2);</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <f t="shared" si="4"/>
+        <v>382</v>
+      </c>
+      <c r="B53">
+        <f>B52</f>
+        <v>95</v>
+      </c>
+      <c r="C53" s="4">
+        <v>678</v>
+      </c>
+      <c r="D53" s="4">
+        <v>0</v>
+      </c>
+      <c r="E53" s="5">
+        <v>0</v>
+      </c>
+      <c r="F53" s="4">
+        <v>1</v>
+      </c>
+      <c r="G53" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (382, 95, 678, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
+        <f t="shared" si="4"/>
+        <v>383</v>
+      </c>
+      <c r="B54">
+        <f>B52</f>
+        <v>95</v>
+      </c>
+      <c r="C54" s="4">
+        <v>679</v>
+      </c>
+      <c r="D54" s="4">
+        <v>1</v>
+      </c>
+      <c r="E54" s="5">
+        <v>0</v>
+      </c>
+      <c r="F54" s="4">
+        <v>2</v>
+      </c>
+      <c r="G54" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (383, 95, 679, 1, 0, 2);</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
+        <f t="shared" si="4"/>
+        <v>384</v>
+      </c>
+      <c r="B55">
+        <f>B52</f>
+        <v>95</v>
+      </c>
+      <c r="C55" s="4">
+        <v>679</v>
+      </c>
+      <c r="D55" s="4">
+        <v>0</v>
+      </c>
+      <c r="E55" s="5">
+        <v>0</v>
+      </c>
+      <c r="F55" s="4">
+        <v>1</v>
+      </c>
+      <c r="G55" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (384, 95, 679, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
+        <f t="shared" si="4"/>
+        <v>385</v>
+      </c>
+      <c r="B56" s="3">
+        <f>B52+1</f>
+        <v>96</v>
+      </c>
+      <c r="C56" s="3">
+        <v>64</v>
+      </c>
+      <c r="D56" s="3">
+        <v>3</v>
+      </c>
+      <c r="E56" s="3">
+        <v>3</v>
+      </c>
+      <c r="F56" s="3">
+        <v>2</v>
+      </c>
+      <c r="G56" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (385, 96, 64, 3, 3, 2);</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="3">
+        <f t="shared" si="4"/>
+        <v>386</v>
+      </c>
+      <c r="B57" s="3">
+        <f>B56</f>
+        <v>96</v>
+      </c>
+      <c r="C57" s="3">
+        <v>64</v>
+      </c>
+      <c r="D57" s="3">
+        <v>0</v>
+      </c>
+      <c r="E57" s="3">
+        <v>0</v>
+      </c>
+      <c r="F57" s="3">
+        <v>1</v>
+      </c>
+      <c r="G57" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (386, 96, 64, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="3">
+        <f t="shared" si="4"/>
+        <v>387</v>
+      </c>
+      <c r="B58" s="3">
+        <f>B56</f>
+        <v>96</v>
+      </c>
+      <c r="C58" s="3">
+        <v>687</v>
+      </c>
+      <c r="D58" s="3">
+        <v>0</v>
+      </c>
+      <c r="E58" s="3">
+        <v>0</v>
+      </c>
+      <c r="F58" s="3">
+        <v>2</v>
+      </c>
+      <c r="G58" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (387, 96, 687, 0, 0, 2);</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="3">
+        <f t="shared" si="4"/>
+        <v>388</v>
+      </c>
+      <c r="B59" s="3">
+        <f>B56</f>
+        <v>96</v>
+      </c>
+      <c r="C59" s="3">
+        <v>687</v>
+      </c>
+      <c r="D59" s="3">
+        <v>0</v>
+      </c>
+      <c r="E59" s="3">
+        <v>0</v>
+      </c>
+      <c r="F59" s="3">
+        <v>1</v>
+      </c>
+      <c r="G59" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (388, 96, 687, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="4">
+        <f t="shared" si="4"/>
+        <v>389</v>
+      </c>
+      <c r="B60">
+        <f>B56+1</f>
+        <v>97</v>
+      </c>
+      <c r="C60" s="4">
+        <v>64</v>
+      </c>
+      <c r="D60" s="4">
+        <v>0</v>
+      </c>
+      <c r="E60" s="5">
+        <v>0</v>
+      </c>
+      <c r="F60" s="4">
+        <v>2</v>
+      </c>
+      <c r="G60" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (389, 97, 64, 0, 0, 2);</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="4">
+        <f t="shared" si="4"/>
+        <v>390</v>
+      </c>
+      <c r="B61">
+        <f>B60</f>
+        <v>97</v>
+      </c>
+      <c r="C61" s="4">
+        <v>64</v>
+      </c>
+      <c r="D61" s="4">
+        <v>0</v>
+      </c>
+      <c r="E61" s="5">
+        <v>0</v>
+      </c>
+      <c r="F61" s="4">
+        <v>1</v>
+      </c>
+      <c r="G61" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (390, 97, 64, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="4">
+        <f t="shared" si="4"/>
+        <v>391</v>
+      </c>
+      <c r="B62">
+        <f>B60</f>
+        <v>97</v>
+      </c>
+      <c r="C62" s="4">
+        <v>679</v>
+      </c>
+      <c r="D62" s="4">
+        <v>2</v>
+      </c>
+      <c r="E62" s="5">
+        <v>3</v>
+      </c>
+      <c r="F62" s="4">
+        <v>2</v>
+      </c>
+      <c r="G62" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (391, 97, 679, 2, 3, 2);</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="4">
+        <f t="shared" si="4"/>
+        <v>392</v>
+      </c>
+      <c r="B63">
+        <f>B60</f>
+        <v>97</v>
+      </c>
+      <c r="C63" s="4">
+        <v>679</v>
+      </c>
+      <c r="D63" s="4">
+        <v>0</v>
+      </c>
+      <c r="E63" s="5">
+        <v>0</v>
+      </c>
+      <c r="F63" s="4">
+        <v>1</v>
+      </c>
+      <c r="G63" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (392, 97, 679, 0, 0, 1);</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>